<commit_message>
corregir funcionalidades de las vista de usuario
</commit_message>
<xml_diff>
--- a/Entrega/assets/Bd-ini.xlsx
+++ b/Entrega/assets/Bd-ini.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Matrix/SynologyDrive/Coderhouse/backend/Entregas-backend/entregas/44-Entrega/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Matrix/SynologyDrive/Coderhouse/backend/Entregas-backend/entregas/Entrega/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6183D31-E224-CC4F-8B0F-D7D94B5A61D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DA97D5-35B2-C247-9E10-40FFCA93181C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{D075B245-05AB-F143-A65C-EAA9F3581B28}"/>
+    <workbookView xWindow="33340" yWindow="5300" windowWidth="36500" windowHeight="18220" activeTab="1" xr2:uid="{D075B245-05AB-F143-A65C-EAA9F3581B28}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -37,19 +37,371 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve"> </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jhon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe </t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Ferreira</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>00000002</t>
+  </si>
+  <si>
+    <t>00000003</t>
+  </si>
+  <si>
+    <t>00000004</t>
+  </si>
+  <si>
+    <t>00000005</t>
+  </si>
+  <si>
+    <t>00000006</t>
+  </si>
+  <si>
+    <t>00000007</t>
+  </si>
+  <si>
+    <t>00000008</t>
+  </si>
+  <si>
+    <t>00000009</t>
+  </si>
+  <si>
+    <t>00000010</t>
+  </si>
+  <si>
+    <t>00000011</t>
+  </si>
+  <si>
+    <t>00000012</t>
+  </si>
+  <si>
+    <t>mail01@mail.com</t>
+  </si>
+  <si>
+    <t>Calle Final 01</t>
+  </si>
+  <si>
+    <t>Calle Final 02</t>
+  </si>
+  <si>
+    <t>Calle Final 03</t>
+  </si>
+  <si>
+    <t>Calle Final 04</t>
+  </si>
+  <si>
+    <t>Calle Final 05</t>
+  </si>
+  <si>
+    <t>Calle Final 06</t>
+  </si>
+  <si>
+    <t>Calle Final 07</t>
+  </si>
+  <si>
+    <t>Calle Final 08</t>
+  </si>
+  <si>
+    <t>Calle Final 09</t>
+  </si>
+  <si>
+    <t>Calle Final 10</t>
+  </si>
+  <si>
+    <t>Calle Final 11</t>
+  </si>
+  <si>
+    <t>Calle Final 12</t>
+  </si>
+  <si>
+    <t>avatar.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan </t>
+  </si>
+  <si>
+    <t>Francisco Carro-Casal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamed </t>
+  </si>
+  <si>
+    <t>Vilanova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carmina </t>
+  </si>
+  <si>
+    <t>Boix Diaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purificación </t>
+  </si>
+  <si>
+    <t>Villalonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eleuterio </t>
+  </si>
+  <si>
+    <t>Ramos Gutierrez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leocadia </t>
+  </si>
+  <si>
+    <t>Aroca-Carro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calixto </t>
+  </si>
+  <si>
+    <t>Zabaleta Izquierdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cecilia </t>
+  </si>
+  <si>
+    <t>Coloma Cerdán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baudelio </t>
+  </si>
+  <si>
+    <t>Bonet Dalmau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albert </t>
+  </si>
+  <si>
+    <t>Moisés Salmerón Seco</t>
+  </si>
+  <si>
+    <t>toximosi@gmail.com</t>
+  </si>
+  <si>
+    <t>mail02@mail.com</t>
+  </si>
+  <si>
+    <t>mail03@mail.com</t>
+  </si>
+  <si>
+    <t>mail04@mail.com</t>
+  </si>
+  <si>
+    <t>mail05@mail.com</t>
+  </si>
+  <si>
+    <t>mail06@mail.com</t>
+  </si>
+  <si>
+    <t>mail07@mail.com</t>
+  </si>
+  <si>
+    <t>mail08@mail.com</t>
+  </si>
+  <si>
+    <t>mail09@mail.com</t>
+  </si>
+  <si>
+    <t>mail10@mail.com</t>
+  </si>
+  <si>
+    <t>mail11@mail.com</t>
+  </si>
+  <si>
+    <t>mail12@mail.com</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>Calle Final 00</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>offer</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>product.png</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>product 01</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aliquam tristique mauris ultricies varius finibus.</t>
+  </si>
+  <si>
+    <t>000002</t>
+  </si>
+  <si>
+    <t>product 02</t>
+  </si>
+  <si>
+    <t>000003</t>
+  </si>
+  <si>
+    <t>product 03</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>product 04</t>
+  </si>
+  <si>
+    <t>000005</t>
+  </si>
+  <si>
+    <t>product 05</t>
+  </si>
+  <si>
+    <t>000006</t>
+  </si>
+  <si>
+    <t>product 06</t>
+  </si>
+  <si>
+    <t>000007</t>
+  </si>
+  <si>
+    <t>product 07</t>
+  </si>
+  <si>
+    <t>000008</t>
+  </si>
+  <si>
+    <t>product 08</t>
+  </si>
+  <si>
+    <t>000009</t>
+  </si>
+  <si>
+    <t>product 09</t>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>product 10</t>
+  </si>
+  <si>
+    <t>000011</t>
+  </si>
+  <si>
+    <t>product 11</t>
+  </si>
+  <si>
+    <t>000012</t>
+  </si>
+  <si>
+    <t>product 12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +424,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,30 +758,728 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E04282C-7E3A-4542-8057-58CF0845BE12}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1234</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="8">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="8">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="8">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="8">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="8">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="8">
+        <v>11</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="8">
+        <v>12</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{139EE1B5-151D-2C45-877B-2D0D2FC66CD2}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{AFF0FEF8-2B29-2B45-B0F8-8D12602455EA}"/>
+    <hyperlink ref="D4:D14" r:id="rId3" display="mail01@mail.com" xr:uid="{BC8390FA-03E3-C646-AED0-6B21DA2EE4DB}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{E94B548F-33A5-0848-A175-7FEF8682E139}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{A3F7219E-4C08-104F-A109-FAB8AF439293}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{F1B10130-7A4A-4E43-9857-C4FEA5E49B1B}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{5DF0C2AD-D6A2-1A4E-9673-CEE7AD1D704B}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{0F84D28A-96A5-004C-A181-2038158227AA}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{47004616-347D-3B4A-A0C0-41B9EEAE199A}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{5D1D14E5-55DD-D147-B42B-915CDB819E4A}"/>
+    <hyperlink ref="D11" r:id="rId11" xr:uid="{79EDEBB4-A544-864D-A5AC-3E6C94521618}"/>
+    <hyperlink ref="D12" r:id="rId12" xr:uid="{F0033C39-5652-4B45-A9C4-222C8B5073CC}"/>
+    <hyperlink ref="D13" r:id="rId13" xr:uid="{D13BED5F-B2D3-4D4E-B90B-26DE278879A4}"/>
+    <hyperlink ref="D14" r:id="rId14" xr:uid="{B8CD2A3C-1805-D143-82C1-AD774C26D22C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63CF427-5DE7-644B-BAB3-F3362BC68A74}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="17" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="20" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="21" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>